<commit_message>
Fixed Sprint Backlog Formatting.
</commit_message>
<xml_diff>
--- a/Deliverable_1/Blackbear-Consultants_Deliverable_1_SprintBacklog_1.xlsx
+++ b/Deliverable_1/Blackbear-Consultants_Deliverable_1_SprintBacklog_1.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdullahkarim/Documents/GitHub/Blackbear-Consultants/Deliverable_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6E4E560-426A-CA48-821B-A4382C52A704}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD84776A-DB42-A043-A21F-966FB4981D5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{29D05152-AD15-448E-8A0D-C19F810C4EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Sprint Goal</t>
   </si>
@@ -238,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -263,16 +262,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -611,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC36FCF-9F37-4AC5-B7F3-1DC0EDBEC864}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
@@ -634,37 +625,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -704,76 +695,76 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="11"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="11"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="11"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="11"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="11"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="11"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
       <c r="M8" s="3" t="s">
         <v>2</v>
       </c>
@@ -840,177 +831,33 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="24"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="20"/>
     </row>
     <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
     </row>
     <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E3A477-5022-4EBF-A5F0-EFD4BBDA3FE6}">
-  <dimension ref="A1:N12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="55.33203125" customWidth="1"/>
-    <col min="2" max="2" width="147.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="M8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="M9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="M10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="M11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="M12" s="5"/>
-      <c r="N12" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>